<commit_message>
removed extra cells below data
</commit_message>
<xml_diff>
--- a/data-raw/household-survey.xlsx
+++ b/data-raw/household-survey.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usfedu-my.sharepoint.com/personal/efv_usf_edu/Documents/Accra and Fulbright/Data/Household survey/for owd/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usfedu-my.sharepoint.com/personal/efv_usf_edu/Documents/Data science course/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{5B80CD7A-677D-E648-9FAE-66E1DA153996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{183A8351-3B7B-EC4F-9BC2-7E687172BB36}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{5B80CD7A-677D-E648-9FAE-66E1DA153996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CA9CA50-977C-DB42-A9BA-D20B2559B46E}"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="2320" windowWidth="26840" windowHeight="15940" xr2:uid="{3FE93E77-7D73-E740-9DF2-848FFCC28C25}"/>
+    <workbookView xWindow="3340" yWindow="1920" windowWidth="26840" windowHeight="15940" xr2:uid="{3FE93E77-7D73-E740-9DF2-848FFCC28C25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,28 +33,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -889,10 +867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D92957-A1D7-2741-BC38-FAC53695D23D}">
-  <dimension ref="A1:CL123"/>
+  <dimension ref="A1:CL117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CA1" workbookViewId="0">
-      <selection activeCell="CL1" sqref="CL1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C131" sqref="C131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30885,32 +30863,6 @@
         <v>260</v>
       </c>
     </row>
-    <row r="119" spans="1:90" x14ac:dyDescent="0.2">
-      <c r="AK119" t="str" cm="1">
-        <f t="array" ref="AK119:AK123">_xlfn.UNIQUE(AK2:AK117)</f>
-        <v>commercial_tap</v>
-      </c>
-    </row>
-    <row r="120" spans="1:90" x14ac:dyDescent="0.2">
-      <c r="AK120" t="str">
-        <v>piped_to_home</v>
-      </c>
-    </row>
-    <row r="121" spans="1:90" x14ac:dyDescent="0.2">
-      <c r="AK121" t="str">
-        <v>piped_to_compound</v>
-      </c>
-    </row>
-    <row r="122" spans="1:90" x14ac:dyDescent="0.2">
-      <c r="AK122" t="str">
-        <v>spring_water</v>
-      </c>
-    </row>
-    <row r="123" spans="1:90" x14ac:dyDescent="0.2">
-      <c r="AK123" t="str">
-        <v>borehole</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Delete extra lines below data
</commit_message>
<xml_diff>
--- a/data-raw/household-survey.xlsx
+++ b/data-raw/household-survey.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usfedu-my.sharepoint.com/personal/efv_usf_edu/Documents/Accra and Fulbright/Data/Household survey/for owd/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usfedu-my.sharepoint.com/personal/efv_usf_edu/Documents/Data science course/final bug check/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{5B80CD7A-677D-E648-9FAE-66E1DA153996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{183A8351-3B7B-EC4F-9BC2-7E687172BB36}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{5B80CD7A-677D-E648-9FAE-66E1DA153996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCCC6673-791C-C04D-9890-232434040826}"/>
   <bookViews>
     <workbookView xWindow="2300" yWindow="2320" windowWidth="26840" windowHeight="15940" xr2:uid="{3FE93E77-7D73-E740-9DF2-848FFCC28C25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,28 +33,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -889,10 +867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D92957-A1D7-2741-BC38-FAC53695D23D}">
-  <dimension ref="A1:CL123"/>
+  <dimension ref="A1:CL117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CA1" workbookViewId="0">
-      <selection activeCell="CL1" sqref="CL1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B128" sqref="B128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30885,32 +30863,6 @@
         <v>260</v>
       </c>
     </row>
-    <row r="119" spans="1:90" x14ac:dyDescent="0.2">
-      <c r="AK119" t="str" cm="1">
-        <f t="array" ref="AK119:AK123">_xlfn.UNIQUE(AK2:AK117)</f>
-        <v>commercial_tap</v>
-      </c>
-    </row>
-    <row r="120" spans="1:90" x14ac:dyDescent="0.2">
-      <c r="AK120" t="str">
-        <v>piped_to_home</v>
-      </c>
-    </row>
-    <row r="121" spans="1:90" x14ac:dyDescent="0.2">
-      <c r="AK121" t="str">
-        <v>piped_to_compound</v>
-      </c>
-    </row>
-    <row r="122" spans="1:90" x14ac:dyDescent="0.2">
-      <c r="AK122" t="str">
-        <v>spring_water</v>
-      </c>
-    </row>
-    <row r="123" spans="1:90" x14ac:dyDescent="0.2">
-      <c r="AK123" t="str">
-        <v>borehole</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>